<commit_message>
Updating daily files for July 11
</commit_message>
<xml_diff>
--- a/assets/My_Pitcher_Listing.xlsx
+++ b/assets/My_Pitcher_Listing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27820"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D02BBC-0AE7-4C67-8C6F-14B1D23F3623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F796EE59-5287-4E37-91D6-D4BE31D5EB64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20553" uniqueCount="2918">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20570" uniqueCount="2920">
   <si>
     <t>mlb_name</t>
   </si>
@@ -8788,6 +8788,12 @@
   </si>
   <si>
     <t>Gordon Graceffo</t>
+  </si>
+  <si>
+    <t>Jack Kochanowicz</t>
+  </si>
+  <si>
+    <t>sa3014539</t>
   </si>
 </sst>
 </file>
@@ -9185,11 +9191,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:S1559"/>
+  <dimension ref="A1:S1560"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V216" sqref="V216"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1287" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R1300" sqref="R1300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -70478,6 +70484,15 @@
       <c r="O1300" t="s">
         <v>2620</v>
       </c>
+      <c r="P1300" t="s">
+        <v>1245</v>
+      </c>
+      <c r="Q1300">
+        <v>669358</v>
+      </c>
+      <c r="R1300" t="s">
+        <v>1245</v>
+      </c>
       <c r="S1300" t="s">
         <v>1245</v>
       </c>
@@ -71452,10 +71467,10 @@
         <v>1283</v>
       </c>
       <c r="C1320" t="s">
-        <v>1309</v>
+        <v>1287</v>
       </c>
       <c r="D1320" t="s">
-        <v>1339</v>
+        <v>1317</v>
       </c>
       <c r="E1320" t="s">
         <v>1347</v>
@@ -82911,6 +82926,56 @@
       </c>
       <c r="S1559" t="s">
         <v>2917</v>
+      </c>
+    </row>
+    <row r="1560" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1560" t="s">
+        <v>2918</v>
+      </c>
+      <c r="B1560" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C1560" t="s">
+        <v>1297</v>
+      </c>
+      <c r="D1560" t="s">
+        <v>1327</v>
+      </c>
+      <c r="E1560" t="s">
+        <v>1347</v>
+      </c>
+      <c r="F1560" t="s">
+        <v>1347</v>
+      </c>
+      <c r="H1560" t="s">
+        <v>2919</v>
+      </c>
+      <c r="I1560" t="s">
+        <v>2918</v>
+      </c>
+      <c r="J1560" t="s">
+        <v>1283</v>
+      </c>
+      <c r="K1560" t="s">
+        <v>2918</v>
+      </c>
+      <c r="L1560" t="s">
+        <v>1283</v>
+      </c>
+      <c r="M1560" t="s">
+        <v>2918</v>
+      </c>
+      <c r="P1560" t="s">
+        <v>2918</v>
+      </c>
+      <c r="Q1560">
+        <v>686799</v>
+      </c>
+      <c r="R1560" t="s">
+        <v>2918</v>
+      </c>
+      <c r="S1560" t="s">
+        <v>2918</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating daily files July 24
</commit_message>
<xml_diff>
--- a/assets/My_Pitcher_Listing.xlsx
+++ b/assets/My_Pitcher_Listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A379B99-3438-4FBE-9DA9-5444BFBEC2A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B5766D-1A3D-402B-B0F9-FD4F353D9F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20590" uniqueCount="2922">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20607" uniqueCount="2924">
   <si>
     <t>mlb_name</t>
   </si>
@@ -8800,6 +8800,12 @@
   </si>
   <si>
     <t>sa3016863</t>
+  </si>
+  <si>
+    <t>Chayce McDermott</t>
+  </si>
+  <si>
+    <t>sa3017420</t>
   </si>
 </sst>
 </file>
@@ -9197,11 +9203,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:S1561"/>
+  <dimension ref="A1:S1562"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S1117" sqref="S1117"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1186" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q1200" sqref="Q1200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -65822,10 +65828,10 @@
         <v>1283</v>
       </c>
       <c r="C1199" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="D1199" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="E1199" t="s">
         <v>1346</v>
@@ -65856,6 +65862,15 @@
       </c>
       <c r="N1199">
         <v>1</v>
+      </c>
+      <c r="P1199" t="s">
+        <v>647</v>
+      </c>
+      <c r="Q1199">
+        <v>592662</v>
+      </c>
+      <c r="R1199" t="s">
+        <v>647</v>
       </c>
       <c r="S1199" t="s">
         <v>647</v>
@@ -83056,6 +83071,56 @@
       </c>
       <c r="S1561" t="s">
         <v>2920</v>
+      </c>
+    </row>
+    <row r="1562" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1562" t="s">
+        <v>2922</v>
+      </c>
+      <c r="B1562" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C1562" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D1562" t="s">
+        <v>1321</v>
+      </c>
+      <c r="E1562" t="s">
+        <v>1347</v>
+      </c>
+      <c r="F1562" t="s">
+        <v>1347</v>
+      </c>
+      <c r="H1562" t="s">
+        <v>2923</v>
+      </c>
+      <c r="I1562" t="s">
+        <v>2922</v>
+      </c>
+      <c r="J1562" t="s">
+        <v>1283</v>
+      </c>
+      <c r="K1562" t="s">
+        <v>2922</v>
+      </c>
+      <c r="L1562" t="s">
+        <v>1283</v>
+      </c>
+      <c r="M1562" t="s">
+        <v>2922</v>
+      </c>
+      <c r="P1562" t="s">
+        <v>2922</v>
+      </c>
+      <c r="Q1562">
+        <v>694646</v>
+      </c>
+      <c r="R1562" t="s">
+        <v>2922</v>
+      </c>
+      <c r="S1562" t="s">
+        <v>2922</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating daily files for sept 12
</commit_message>
<xml_diff>
--- a/assets/My_Pitcher_Listing.xlsx
+++ b/assets/My_Pitcher_Listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27163747-0197-440D-B740-90C9247E1AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF49EF51-B10E-47E0-9B46-1F4CE33573C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20858" uniqueCount="2941">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20871" uniqueCount="2942">
   <si>
     <t>mlb_name</t>
   </si>
@@ -8857,6 +8857,9 @@
   </si>
   <si>
     <t>Reynaldo López</t>
+  </si>
+  <si>
+    <t>Kumar Rocker</t>
   </si>
 </sst>
 </file>
@@ -9254,11 +9257,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:S1579"/>
+  <dimension ref="A1:S1580"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1165" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P1178" sqref="P1178"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1556" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q1581" sqref="Q1581"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -84015,8 +84018,8 @@
       <c r="F1578" t="s">
         <v>1347</v>
       </c>
-      <c r="H1578" t="s">
-        <v>2938</v>
+      <c r="H1578">
+        <v>30160</v>
       </c>
       <c r="I1578" t="s">
         <v>2937</v>
@@ -84065,8 +84068,8 @@
       <c r="F1579" t="s">
         <v>1347</v>
       </c>
-      <c r="H1579" t="s">
-        <v>2938</v>
+      <c r="H1579">
+        <v>26020</v>
       </c>
       <c r="I1579" t="s">
         <v>2939</v>
@@ -84094,6 +84097,56 @@
       </c>
       <c r="S1579" t="s">
         <v>2939</v>
+      </c>
+    </row>
+    <row r="1580" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1580" t="s">
+        <v>2941</v>
+      </c>
+      <c r="B1580" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C1580" t="s">
+        <v>1303</v>
+      </c>
+      <c r="D1580" t="s">
+        <v>1333</v>
+      </c>
+      <c r="E1580" t="s">
+        <v>1347</v>
+      </c>
+      <c r="F1580" t="s">
+        <v>1347</v>
+      </c>
+      <c r="H1580" t="s">
+        <v>2938</v>
+      </c>
+      <c r="I1580" t="s">
+        <v>2941</v>
+      </c>
+      <c r="J1580" t="s">
+        <v>1283</v>
+      </c>
+      <c r="K1580" t="s">
+        <v>2941</v>
+      </c>
+      <c r="L1580" t="s">
+        <v>1283</v>
+      </c>
+      <c r="M1580" t="s">
+        <v>2941</v>
+      </c>
+      <c r="P1580" t="s">
+        <v>2941</v>
+      </c>
+      <c r="Q1580">
+        <v>677958</v>
+      </c>
+      <c r="R1580" t="s">
+        <v>2941</v>
+      </c>
+      <c r="S1580" t="s">
+        <v>2941</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating daily files for sept 13
</commit_message>
<xml_diff>
--- a/assets/My_Pitcher_Listing.xlsx
+++ b/assets/My_Pitcher_Listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF49EF51-B10E-47E0-9B46-1F4CE33573C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81E6BF1-B053-4094-A8B1-F9E2F1B1A767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20871" uniqueCount="2942">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20886" uniqueCount="2942">
   <si>
     <t>mlb_name</t>
   </si>
@@ -8850,9 +8850,6 @@
     <t>Richard Fitts</t>
   </si>
   <si>
-    <t>sa123</t>
-  </si>
-  <si>
     <t>Seth Johnson</t>
   </si>
   <si>
@@ -8860,6 +8857,9 @@
   </si>
   <si>
     <t>Kumar Rocker</t>
+  </si>
+  <si>
+    <t>Brady Basso</t>
   </si>
 </sst>
 </file>
@@ -9257,11 +9257,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:S1580"/>
+  <dimension ref="A1:S1581"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1556" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q1581" sqref="Q1581"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1557" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q1582" sqref="Q1582"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -38382,10 +38382,10 @@
         <v>1283</v>
       </c>
       <c r="C619" t="s">
-        <v>1315</v>
+        <v>1303</v>
       </c>
       <c r="D619" t="s">
-        <v>1345</v>
+        <v>1333</v>
       </c>
       <c r="E619" t="s">
         <v>1346</v>
@@ -38416,6 +38416,15 @@
       </c>
       <c r="N619">
         <v>1</v>
+      </c>
+      <c r="P619" t="s">
+        <v>331</v>
+      </c>
+      <c r="Q619">
+        <v>594798</v>
+      </c>
+      <c r="R619" t="s">
+        <v>331</v>
       </c>
       <c r="S619" t="s">
         <v>331</v>
@@ -64985,13 +64994,13 @@
         <v>1</v>
       </c>
       <c r="P1178" t="s">
-        <v>2940</v>
+        <v>2939</v>
       </c>
       <c r="Q1178">
         <v>625643</v>
       </c>
       <c r="R1178" t="s">
-        <v>2940</v>
+        <v>2939</v>
       </c>
       <c r="S1178" t="s">
         <v>637</v>
@@ -84051,7 +84060,7 @@
     </row>
     <row r="1579" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1579" t="s">
-        <v>2939</v>
+        <v>2938</v>
       </c>
       <c r="B1579" t="s">
         <v>1283</v>
@@ -84072,36 +84081,36 @@
         <v>26020</v>
       </c>
       <c r="I1579" t="s">
-        <v>2939</v>
+        <v>2938</v>
       </c>
       <c r="J1579" t="s">
         <v>1283</v>
       </c>
       <c r="K1579" t="s">
-        <v>2939</v>
+        <v>2938</v>
       </c>
       <c r="L1579" t="s">
         <v>1283</v>
       </c>
       <c r="M1579" t="s">
-        <v>2939</v>
+        <v>2938</v>
       </c>
       <c r="P1579" t="s">
-        <v>2939</v>
+        <v>2938</v>
       </c>
       <c r="Q1579">
         <v>686751</v>
       </c>
       <c r="R1579" t="s">
-        <v>2939</v>
+        <v>2938</v>
       </c>
       <c r="S1579" t="s">
-        <v>2939</v>
+        <v>2938</v>
       </c>
     </row>
     <row r="1580" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1580" t="s">
-        <v>2941</v>
+        <v>2940</v>
       </c>
       <c r="B1580" t="s">
         <v>1283</v>
@@ -84118,34 +84127,84 @@
       <c r="F1580" t="s">
         <v>1347</v>
       </c>
-      <c r="H1580" t="s">
-        <v>2938</v>
+      <c r="H1580">
+        <v>31843</v>
       </c>
       <c r="I1580" t="s">
-        <v>2941</v>
+        <v>2940</v>
       </c>
       <c r="J1580" t="s">
         <v>1283</v>
       </c>
       <c r="K1580" t="s">
-        <v>2941</v>
+        <v>2940</v>
       </c>
       <c r="L1580" t="s">
         <v>1283</v>
       </c>
       <c r="M1580" t="s">
-        <v>2941</v>
+        <v>2940</v>
       </c>
       <c r="P1580" t="s">
-        <v>2941</v>
+        <v>2940</v>
       </c>
       <c r="Q1580">
         <v>677958</v>
       </c>
       <c r="R1580" t="s">
+        <v>2940</v>
+      </c>
+      <c r="S1580" t="s">
+        <v>2940</v>
+      </c>
+    </row>
+    <row r="1581" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1581" t="s">
         <v>2941</v>
       </c>
-      <c r="S1580" t="s">
+      <c r="B1581" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C1581" t="s">
+        <v>1289</v>
+      </c>
+      <c r="D1581" t="s">
+        <v>1319</v>
+      </c>
+      <c r="E1581" t="s">
+        <v>1346</v>
+      </c>
+      <c r="F1581" t="s">
+        <v>1346</v>
+      </c>
+      <c r="H1581">
+        <v>25582</v>
+      </c>
+      <c r="I1581" t="s">
+        <v>2941</v>
+      </c>
+      <c r="J1581" t="s">
+        <v>1283</v>
+      </c>
+      <c r="K1581" t="s">
+        <v>2941</v>
+      </c>
+      <c r="L1581" t="s">
+        <v>1283</v>
+      </c>
+      <c r="M1581" t="s">
+        <v>2941</v>
+      </c>
+      <c r="P1581" t="s">
+        <v>2941</v>
+      </c>
+      <c r="Q1581">
+        <v>669620</v>
+      </c>
+      <c r="R1581" t="s">
+        <v>2941</v>
+      </c>
+      <c r="S1581" t="s">
         <v>2941</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating files and app
</commit_message>
<xml_diff>
--- a/assets/My_Pitcher_Listing.xlsx
+++ b/assets/My_Pitcher_Listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94567CCD-EAEC-4E9F-91E0-72A7A9822270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{041E2BFC-7A51-420D-86D6-C0D0866D1684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26241,11 +26241,11 @@
         <v>20</v>
       </c>
       <c r="C324" t="s">
-        <v>41</v>
+        <v>118</v>
       </c>
       <c r="D324" t="str">
         <f>VLOOKUP(Players!C324,Teams!A:B,2,FALSE)</f>
-        <v>Milwaukee Brewers</v>
+        <v>Chicago Cubs</v>
       </c>
       <c r="E324" t="s">
         <v>23</v>
@@ -26285,7 +26285,7 @@
       </c>
       <c r="T324" t="str">
         <f>VLOOKUP(C324,Teams!$A$1:$C$31,3,FALSE)</f>
-        <v>Milwaukee</v>
+        <v>Chicago</v>
       </c>
     </row>
     <row r="325" spans="1:20" x14ac:dyDescent="0.3">

</xml_diff>